<commit_message>
Fix dynamic onto class creation
</commit_message>
<xml_diff>
--- a/data/warehouse_data_v2.xlsx
+++ b/data/warehouse_data_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Warehouse overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="250">
   <si>
     <t xml:space="preserve">[0,0]</t>
   </si>
@@ -769,6 +769,12 @@
   </si>
   <si>
     <t xml:space="preserve">inbound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.2019</t>
   </si>
 </sst>
 </file>
@@ -1147,10 +1153,10 @@
   <dimension ref="B4:AC21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z4" activeCellId="0" sqref="Z4"/>
+      <selection pane="topLeft" activeCell="Z4" activeCellId="1" sqref="D7:F7 Z4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.28"/>
@@ -1161,7 +1167,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8"/>
@@ -1169,7 +1175,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="14.69"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,12 +1988,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="D7:F7 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,18 +2098,18 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1048556" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1048576" activeCellId="0" sqref="J1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1048576" activeCellId="1" sqref="D7:F7 J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.86"/>
   </cols>
@@ -2304,10 +2310,10 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI2" activeCellId="0" sqref="AI2"/>
+      <selection pane="topLeft" activeCell="AI2" activeCellId="1" sqref="D7:F7 AI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.57"/>
@@ -2315,11 +2321,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28.57"/>
   </cols>
@@ -2557,20 +2563,20 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="M14" activeCellId="1" sqref="D7:F7 M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,6 +2637,9 @@
         <v>3000</v>
       </c>
       <c r="I2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -2652,13 +2661,13 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.01"/>
@@ -2879,12 +2888,18 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>247</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>249</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>231</v>

</xml_diff>